<commit_message>
modified:   actual_items.xlsx 	modified:   report.pbix 	modified:   stock_analysis.ipynb 	modified:   stock_analysis.xlsx 	modified:   stock_analysis_final.xlsx 	modified:   time_series_10_22.pkl
</commit_message>
<xml_diff>
--- a/stock_analysis.xlsx
+++ b/stock_analysis.xlsx
@@ -472,16 +472,18 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>254</v>
+        <v>134</v>
       </c>
       <c r="D2" t="n">
         <v>81632</v>
       </c>
       <c r="E2" t="n">
-        <v>74</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
+        <v>199</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2023-05-09</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -1854,7 +1856,7 @@
         <v>9750</v>
       </c>
       <c r="E55" t="n">
-        <v>104</v>
+        <v>1365</v>
       </c>
       <c r="F55" t="n">
         <v>0</v>

</xml_diff>